<commit_message>
Added two more exercises
</commit_message>
<xml_diff>
--- a/Spreadsheets/Traffic Light Delay Simulator.xlsx
+++ b/Spreadsheets/Traffic Light Delay Simulator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="690" windowWidth="21600" windowHeight="10260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1035" windowWidth="21600" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -8000,7 +8000,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="1"/>
-            <a:t>Generating an Exponential Distribution</a:t>
+            <a:t>1. Generating an Exponential Distribution</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -8216,7 +8216,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200" b="1"/>
-            <a:t>Generating an Weibull/Rayleigh Distribution</a:t>
+            <a:t>2. Generating an Weibull/Rayleigh Distribution</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -8640,6 +8640,473 @@
         <a:xfrm>
           <a:off x="7610475" y="2838450"/>
           <a:ext cx="9734550" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Delete this square to see the solution</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> and discussion below</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>255059</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83608</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>74084</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10023587-4168-47E7-8AFD-571C1396BF96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="255059" y="5626100"/>
+          <a:ext cx="4125382" cy="924984"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>3. Does the order of delays impact the distribution?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:t>Set the inputs values and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0"/>
+            <a:t> try and get a left-skewed distribution (tail on the left side, peak on the right). Can you do it?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>222249</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>99484</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24D47B1E-43C4-4C14-B8F4-395ED5E2B143}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7873999" y="5461000"/>
+          <a:ext cx="6466417" cy="924984"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:t>No, the final cycle-time is the sum of the delays. Just like 1 + 3 + 5 is identical to 5 + 3 + 1.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:t>In fact, different delays will impact each car or piece of work,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0"/>
+            <a:t> so its not important the order or what delays, just that there are delays at all. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>307976</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>97368</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>158751</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFDA4859-6BBE-49DF-BF64-3F7CAF2E20F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7673976" y="5240868"/>
+          <a:ext cx="6931024" cy="1394883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Delete this square to see the solution</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> and discussion below</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>269876</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>105831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>98425</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>95248</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF06FBA-E207-47B9-97A0-712C765FECAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="269876" y="6773331"/>
+          <a:ext cx="4125382" cy="1132417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>4. Does work time impact distribution shape?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:t>Double the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0"/>
+            <a:t> base travel time and halve the delay times. what happens to the distribution shape? Make sure you watch the X-Axis values.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>513292</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>126998</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>99482</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCCBB5FA-E8BC-4213-B31B-2EB5F80DFB3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7879292" y="6794498"/>
+          <a:ext cx="6249457" cy="924984"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0"/>
+            <a:t>No, the distribution is based on how the delays combine. The length of work alters</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0"/>
+            <a:t> the scale of the cycle time, not the shape. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>322793</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>69852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>131235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{578A3528-BD1E-420E-B0BB-18A6CFF64A8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7688793" y="6737352"/>
+          <a:ext cx="6931024" cy="1394883"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9526,7 +9993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -9550,6 +10017,21 @@
       <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="36">
+        <v>0.2</v>
+      </c>
+    </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" s="36">
         <v>0.2</v>
@@ -9581,7 +10063,7 @@
   <dimension ref="A1:AN39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11003,8 +11485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>